<commit_message>
New graph for the LCIA of IGUs, see 02_LCA
</commit_message>
<xml_diff>
--- a/files/lci_spacers.xlsx
+++ b/files/lci_spacers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souvi\Documents\These\80_Calculations\05_LCA\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB40AE7F-E525-4B09-A2A5-B579C27DCFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82446477-D364-4F4C-8260-82F92A433A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="818" firstSheet="5" activeTab="13" xr2:uid="{B87BFFB3-3456-42B2-AA1B-272EE0BB9BDB}"/>
+    <workbookView xWindow="30" yWindow="930" windowWidth="28770" windowHeight="15270" tabRatio="818" firstSheet="5" activeTab="13" xr2:uid="{B87BFFB3-3456-42B2-AA1B-272EE0BB9BDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hypothesis" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2956" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2890" uniqueCount="215">
   <si>
     <t>skip</t>
   </si>
@@ -4726,10 +4726,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C1C0AA4-0B10-4B66-8BB8-AF921BB03436}">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5011,272 +5011,49 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>92</v>
-      </c>
-      <c r="B14" s="21">
-        <v>0.99639999999999995</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>64</v>
+      <c r="A14" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="B14" s="17">
+        <v>1</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>166</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="L14" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="M14" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="N14" s="12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B15" s="24">
-        <v>2.3913600000000001E-4</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="J15" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="K15" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="L15" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="M15" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="N15" s="19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>83</v>
-      </c>
-      <c r="B16" s="21">
-        <v>3.2094</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="12" t="s">
+      <c r="F14" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="K16" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="L16" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="M16" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="N16" s="12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="B17" s="17">
-        <v>1</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="G17" s="17" t="s">
+      <c r="G14" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="H17" s="17">
+      <c r="H14" s="17">
         <v>2</v>
       </c>
-      <c r="I17" s="17">
+      <c r="I14" s="17">
         <v>-1.427</v>
       </c>
-      <c r="J17" s="17">
+      <c r="J14" s="17">
         <v>0.30335622624234998</v>
       </c>
-      <c r="K17" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="L17" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="M17" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="N17" s="17" t="s">
+      <c r="K14" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="M14" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="N14" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="O17" s="22"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>86</v>
-      </c>
-      <c r="B18" s="21">
-        <v>-9.9639999999999993E-4</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="H18" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="I18" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="J18" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="K18" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="L18" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="M18" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="N18" s="12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B19" s="21">
-        <v>-1.3556999999999999</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="H19" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="I19" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="J19" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="K19" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="L19" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="M19" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="N19" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="O19" s="28" t="s">
-        <v>76</v>
-      </c>
+      <c r="O14" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>